<commit_message>
- minor mods to support/build.sh so that command generator will be run ONLY if the gradle process exits normally - Excel: handles OLE2NotOfficeXmlFileException when attempting to open a XLS file as a Excel-2007 format - Nexial Filter: reordered NexialFilterComparator to improve REGEX search & group - adding org.junit.runners.ParentRunner as another class to signify current environment as "unit testing" (and thus disable console interaction) - fixed failed tests
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_base_macro2.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_base_macro2.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39345014-80ED-454D-A671-D1A72F4CF0DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F70BA5-5302-904E-86CB-26E9D7DD5421}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27320" yWindow="440" windowWidth="13640" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,20 +54,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -117,6 +111,45 @@
   </si>
   <si>
     <t>1.6</t>
+  </si>
+  <si>
+    <t>23.95</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>43.84</t>
+  </si>
+  <si>
+    <t>calc-expected-3</t>
+  </si>
+  <si>
+    <t>calc-expected-1</t>
+  </si>
+  <si>
+    <t>13.625</t>
+  </si>
+  <si>
+    <t>calc-expected-2</t>
+  </si>
+  <si>
+    <t>2.1875</t>
+  </si>
+  <si>
+    <t>calc-expected-4</t>
+  </si>
+  <si>
+    <t>calc-expected-5</t>
+  </si>
+  <si>
+    <t>22.4</t>
+  </si>
+  <si>
+    <t>9.5</t>
   </si>
 </sst>
 </file>
@@ -600,15 +633,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA11"/>
+  <dimension ref="A1:AAA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -617,7 +650,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -627,57 +660,57 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -687,43 +720,95 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -739,7 +824,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B16:B1048576 B1:B14">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>

</xml_diff>